<commit_message>
started converting com files
</commit_message>
<xml_diff>
--- a/DFT_Calculations/convert_to_open_shell/smiles_with_mapping.xlsx
+++ b/DFT_Calculations/convert_to_open_shell/smiles_with_mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R9000P\stahl_data_science\DFT_Calculations\smiles_to_log\working_dir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R9000P\stahl_data_science\DFT_Calculations\convert_to_open_shell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705ED285-AC6C-46F4-9DAD-86B76D48EEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026AB026-4F77-480E-8C5A-762E2BB4AB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{A3D57890-EAF1-9348-A434-A2696BF9CCF6}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="17145" xr2:uid="{A3D57890-EAF1-9348-A434-A2696BF9CCF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
     <t>CCC1=C2C=CC=CC2=NC=N1</t>
   </si>
   <si>
-    <t>Mapping</t>
+    <t>mapping</t>
   </si>
 </sst>
 </file>
@@ -766,13 +766,14 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="11.25" style="2"/>
+    <col min="2" max="3" width="11.25" style="2"/>
+    <col min="5" max="16384" width="11.25" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>